<commit_message>
Added Supp table 3
</commit_message>
<xml_diff>
--- a/Sup_Final Assigment.xlsx
+++ b/Sup_Final Assigment.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giang nguyen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sushmaambekar/Documents/GitHub/BCB546--FINAL-GROUP-PROJECT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17292E00-C91B-418F-8715-9F5B222E56C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33835E47-A8DF-2E4B-8286-496D77B9F64F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4527CE78-878C-426E-B047-32FD52F89D26}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{4527CE78-878C-426E-B047-32FD52F89D26}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplementary Table 1" sheetId="1" r:id="rId1"/>
     <sheet name="Supplementary Table 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Supplementary Table 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="230">
   <si>
     <t>Population</t>
   </si>
@@ -410,6 +411,321 @@
   </si>
   <si>
     <t xml:space="preserve">Lineage 1 </t>
+  </si>
+  <si>
+    <t>katG</t>
+  </si>
+  <si>
+    <t>S315T</t>
+  </si>
+  <si>
+    <t>rpoB</t>
+  </si>
+  <si>
+    <t>S450L</t>
+  </si>
+  <si>
+    <t>rpsL</t>
+  </si>
+  <si>
+    <t>K43R</t>
+  </si>
+  <si>
+    <t>embB</t>
+  </si>
+  <si>
+    <t>M306V</t>
+  </si>
+  <si>
+    <t>M306I</t>
+  </si>
+  <si>
+    <t>Rv1482c-fabG1</t>
+  </si>
+  <si>
+    <t>C-15T</t>
+  </si>
+  <si>
+    <t>rrs</t>
+  </si>
+  <si>
+    <t>A1401G</t>
+  </si>
+  <si>
+    <t>A514C</t>
+  </si>
+  <si>
+    <t>gyrA</t>
+  </si>
+  <si>
+    <t>A90V</t>
+  </si>
+  <si>
+    <t>D94G</t>
+  </si>
+  <si>
+    <t>gid</t>
+  </si>
+  <si>
+    <t>L79S</t>
+  </si>
+  <si>
+    <t>L452P</t>
+  </si>
+  <si>
+    <t>ethA-ethR</t>
+  </si>
+  <si>
+    <t>T-65C</t>
+  </si>
+  <si>
+    <t>T-8A</t>
+  </si>
+  <si>
+    <t>D435V</t>
+  </si>
+  <si>
+    <t>D435G</t>
+  </si>
+  <si>
+    <t>ubiA</t>
+  </si>
+  <si>
+    <t>V188A</t>
+  </si>
+  <si>
+    <t>I1106T</t>
+  </si>
+  <si>
+    <t>inhA</t>
+  </si>
+  <si>
+    <t>S94A</t>
+  </si>
+  <si>
+    <t>G-17T</t>
+  </si>
+  <si>
+    <t>I194T</t>
+  </si>
+  <si>
+    <t>A249T</t>
+  </si>
+  <si>
+    <t>PPE52-nuoA</t>
+  </si>
+  <si>
+    <t>G-314T</t>
+  </si>
+  <si>
+    <t>eis-Rv2417c</t>
+  </si>
+  <si>
+    <t>C-10T</t>
+  </si>
+  <si>
+    <t>K88R</t>
+  </si>
+  <si>
+    <t>iniA</t>
+  </si>
+  <si>
+    <t>H42R</t>
+  </si>
+  <si>
+    <t>D94A</t>
+  </si>
+  <si>
+    <t>alr</t>
+  </si>
+  <si>
+    <t>L113R</t>
+  </si>
+  <si>
+    <t>pncA</t>
+  </si>
+  <si>
+    <t>Q10*</t>
+  </si>
+  <si>
+    <t>Q497R</t>
+  </si>
+  <si>
+    <t>D435Y</t>
+  </si>
+  <si>
+    <t>H445Y</t>
+  </si>
+  <si>
+    <t>S91P</t>
+  </si>
+  <si>
+    <t>Gene / Intergenic region</t>
+  </si>
+  <si>
+    <t>Mutation</t>
+  </si>
+  <si>
+    <t>Susceptible %</t>
+  </si>
+  <si>
+    <t>DR %</t>
+  </si>
+  <si>
+    <t>MDR-TB allele frequency %</t>
+  </si>
+  <si>
+    <t>XDR-TB allele frequency %</t>
+  </si>
+  <si>
+    <t>embC-embA</t>
+  </si>
+  <si>
+    <t>C-12T</t>
+  </si>
+  <si>
+    <t>G406A</t>
+  </si>
+  <si>
+    <t>Q10P</t>
+  </si>
+  <si>
+    <t>G-12A</t>
+  </si>
+  <si>
+    <t>C-16T</t>
+  </si>
+  <si>
+    <t>C-16G</t>
+  </si>
+  <si>
+    <t>H445D</t>
+  </si>
+  <si>
+    <t>D94Y</t>
+  </si>
+  <si>
+    <t>thyX-hsdS.1</t>
+  </si>
+  <si>
+    <t>G-16A</t>
+  </si>
+  <si>
+    <t>L731P</t>
+  </si>
+  <si>
+    <t>G406D</t>
+  </si>
+  <si>
+    <t>V125G</t>
+  </si>
+  <si>
+    <t>C-11A</t>
+  </si>
+  <si>
+    <t>S315R</t>
+  </si>
+  <si>
+    <t>pncA-Rv2044c</t>
+  </si>
+  <si>
+    <t>T-11C</t>
+  </si>
+  <si>
+    <t>S315N</t>
+  </si>
+  <si>
+    <t>D94N</t>
+  </si>
+  <si>
+    <t>M423T</t>
+  </si>
+  <si>
+    <t>A80P</t>
+  </si>
+  <si>
+    <t>G-43C</t>
+  </si>
+  <si>
+    <t>D354A</t>
+  </si>
+  <si>
+    <t>Rv2172c-idsA2</t>
+  </si>
+  <si>
+    <t>A-65G</t>
+  </si>
+  <si>
+    <t>C-12A</t>
+  </si>
+  <si>
+    <t>P397T</t>
+  </si>
+  <si>
+    <t>C517T</t>
+  </si>
+  <si>
+    <t>G-14A</t>
+  </si>
+  <si>
+    <t>G406S</t>
+  </si>
+  <si>
+    <t>H445R</t>
+  </si>
+  <si>
+    <t>D1024N</t>
+  </si>
+  <si>
+    <t>oxyR’-ahpC</t>
+  </si>
+  <si>
+    <t>G-48A</t>
+  </si>
+  <si>
+    <t>M343T</t>
+  </si>
+  <si>
+    <t>S450W</t>
+  </si>
+  <si>
+    <t>C-52T</t>
+  </si>
+  <si>
+    <t>H445L</t>
+  </si>
+  <si>
+    <t>V139M</t>
+  </si>
+  <si>
+    <t>H445N</t>
+  </si>
+  <si>
+    <t>L430P</t>
+  </si>
+  <si>
+    <t>C-8T</t>
+  </si>
+  <si>
+    <t>I491F</t>
+  </si>
+  <si>
+    <t>W68*</t>
+  </si>
+  <si>
+    <t>T-8C</t>
+  </si>
+  <si>
+    <t>Q141P</t>
+  </si>
+  <si>
+    <t>D94H</t>
+  </si>
+  <si>
+    <t>A514T</t>
+  </si>
+  <si>
+    <t>M434I</t>
   </si>
 </sst>
 </file>
@@ -445,10 +761,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,20 +1084,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4202B2-4482-411B-AEEE-BC875DD8D8F0}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -813,7 +1132,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -848,7 +1167,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -883,7 +1202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -918,7 +1237,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -953,7 +1272,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -988,7 +1307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1023,7 +1342,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1058,7 +1377,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1093,7 +1412,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1128,7 +1447,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1163,7 +1482,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1198,7 +1517,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1233,7 +1552,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1268,7 +1587,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1303,7 +1622,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1338,7 +1657,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1373,7 +1692,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1408,7 +1727,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1443,7 +1762,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1478,7 +1797,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1510,7 +1829,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1555,15 +1874,15 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -1586,7 +1905,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1609,7 +1928,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -1632,7 +1951,7 @@
         <v>27.4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -1655,7 +1974,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -1678,7 +1997,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -1701,7 +2020,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -1724,7 +2043,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>103</v>
       </c>
@@ -1747,7 +2066,7 @@
         <v>25.3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>104</v>
       </c>
@@ -1770,7 +2089,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -1793,7 +2112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>106</v>
       </c>
@@ -1816,7 +2135,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>107</v>
       </c>
@@ -1839,7 +2158,7 @@
         <v>38.9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -1862,7 +2181,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>92</v>
       </c>
@@ -1885,7 +2204,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -1908,7 +2227,7 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -1943,7 +2262,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -1978,7 +2297,7 @@
         <v>68.8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -2013,7 +2332,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -2048,7 +2367,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2087,4 +2406,1608 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F582E4-387C-E749-AC06-F53A2751EC46}">
+  <dimension ref="A1:F79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D2" s="3">
+        <v>36.9</v>
+      </c>
+      <c r="E2" s="3">
+        <v>71.7</v>
+      </c>
+      <c r="F2" s="3">
+        <v>73.400000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>64.2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>56.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>42.2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>31.2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>39.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="F6" s="3">
+        <v>35.200000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>21.9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="F7" s="3">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E8" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>72.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="F9" s="3">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F10" s="3">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F11" s="3">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="F13" s="3">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E14" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F14" s="3">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E15" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="F15" s="3">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E16" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F17" s="3">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>5.7</v>
+      </c>
+      <c r="E20" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F21" s="3">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="E22" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="F22" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F23" s="3">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E25" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="F25" s="3">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D26" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="E26" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="F27" s="3">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F28" s="3">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F29" s="3">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="E31" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E32" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="F32" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="E33" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="F34" s="3">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E35" s="3">
+        <v>3</v>
+      </c>
+      <c r="F35" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E36" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="F36" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="E39" s="3">
+        <v>2</v>
+      </c>
+      <c r="F39" s="3">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F40" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="E41" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="E43" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F43" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="E44" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="F44" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E45" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="F45" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="F46" s="3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F47" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E48" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="F48" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E49" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="F49" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="F50" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F51" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0</v>
+      </c>
+      <c r="D52" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C53" s="3">
+        <v>0</v>
+      </c>
+      <c r="D53" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C54" s="3">
+        <v>0</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="F54" s="3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E55" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C56" s="3">
+        <v>0</v>
+      </c>
+      <c r="D56" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F56" s="3">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C57" s="3">
+        <v>0</v>
+      </c>
+      <c r="D57" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F57" s="3">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C58" s="3">
+        <v>0</v>
+      </c>
+      <c r="D58" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E58" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F58" s="3">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C59" s="3">
+        <v>0</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="F59" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C60" s="3">
+        <v>0</v>
+      </c>
+      <c r="D60" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E60" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F60" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C61" s="3">
+        <v>0</v>
+      </c>
+      <c r="D61" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="E61" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="F61" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C62" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D62" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E62" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C63" s="3">
+        <v>0</v>
+      </c>
+      <c r="D63" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E63" s="3">
+        <v>1</v>
+      </c>
+      <c r="F63" s="3">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C64" s="3">
+        <v>0</v>
+      </c>
+      <c r="D64" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E64" s="3">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C65" s="3">
+        <v>0</v>
+      </c>
+      <c r="D65" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="E65" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F65" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C66" s="3">
+        <v>0</v>
+      </c>
+      <c r="D66" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="E66" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="F66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C67" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D67" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E67" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="F67" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C68" s="3">
+        <v>0</v>
+      </c>
+      <c r="D68" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E68" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="F68" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C69" s="3">
+        <v>0</v>
+      </c>
+      <c r="D69" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E69" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="F69" s="3">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C70" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D70" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="E70" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C71" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D71" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E71" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="F71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C72" s="3">
+        <v>0</v>
+      </c>
+      <c r="D72" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E72" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="F72" s="3">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C73" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D73" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="E73" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F73" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C74" s="3">
+        <v>0</v>
+      </c>
+      <c r="D74" s="3">
+        <v>0</v>
+      </c>
+      <c r="E74" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C75" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D75" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E75" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F75" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C76" s="3">
+        <v>0</v>
+      </c>
+      <c r="D76" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E76" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="F76" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C77" s="3">
+        <v>0</v>
+      </c>
+      <c r="D77" s="3">
+        <v>0</v>
+      </c>
+      <c r="E77" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="F77" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C78" s="3">
+        <v>0</v>
+      </c>
+      <c r="D78" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="E78" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F78" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C79" s="3">
+        <v>0</v>
+      </c>
+      <c r="D79" s="3">
+        <v>0</v>
+      </c>
+      <c r="E79" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F79" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>